<commit_message>
Susan updated Repro Protocol datasheet and made a minor tweak in datasheet data dictionary for repro and primary in num_leaves and num_repro
</commit_message>
<xml_diff>
--- a/forms/HerbVar_Datasheet_Template.xlsx
+++ b/forms/HerbVar_Datasheet_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wetzel/Repos/HerbVar-website/protocols/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B86453AC-F442-CE4D-98F9-767B4C75F857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2052927-4EA9-0842-96E4-089994CC5251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9480" yWindow="740" windowWidth="19920" windowHeight="18380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="siteData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="245">
   <si>
     <t>variable</t>
   </si>
@@ -181,9 +181,6 @@
     <t>numReproHerb</t>
   </si>
   <si>
-    <t>percReproHerb</t>
-  </si>
-  <si>
     <t>percR1</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>size of plant, as specified by plantSizeMetric &amp; plantSizeMetric</t>
   </si>
   <si>
-    <t xml:space="preserve">Total number of leaves on plant individual (including damaged leaves). If plant individual has ~60 leaves or less, count all leaves. If plant individual has more than ~ 60 leaves, count a subsample of ~ 60 random (arbitrarily chosen) leaves.  </t>
-  </si>
-  <si>
     <t>centimeters</t>
   </si>
   <si>
@@ -281,15 +275,6 @@
   </si>
   <si>
     <t>characters</t>
-  </si>
-  <si>
-    <t>b, fl, fr, s</t>
-  </si>
-  <si>
-    <t>type of reproductive structure (bud, flower, fruit, seed)</t>
-  </si>
-  <si>
-    <t>total number of reproductive structures/plant examined (if too many to look at all of them, pick a random subset as for leaves; e.g. N=30)</t>
   </si>
   <si>
     <t>protocolFollowed</t>
@@ -416,21 +401,6 @@
     <t>damageUnit</t>
   </si>
   <si>
-    <t>percR11</t>
-  </si>
-  <si>
-    <t>percR12</t>
-  </si>
-  <si>
-    <t>percR13</t>
-  </si>
-  <si>
-    <t>percR14</t>
-  </si>
-  <si>
-    <t>percR15</t>
-  </si>
-  <si>
     <t>numReproPath</t>
   </si>
   <si>
@@ -464,18 +434,6 @@
     <t>beetleHerbivore</t>
   </si>
   <si>
-    <t>percReproPath</t>
-  </si>
-  <si>
-    <t>percReproChew</t>
-  </si>
-  <si>
-    <t>percReproPierce</t>
-  </si>
-  <si>
-    <t>percReproUnkDmg</t>
-  </si>
-  <si>
     <t>NOTES TO DATA ENTERER:</t>
   </si>
   <si>
@@ -495,9 +453,6 @@
   </si>
   <si>
     <t>This is the place for any notes that apply to the entire survey/data file</t>
-  </si>
-  <si>
-    <t>You do not need to fill out both the num_ and perc_ versions of the same column. Both options are provided for your convenience but the protocol only calls for one or the other</t>
   </si>
   <si>
     <t>percLf15</t>
@@ -734,23 +689,6 @@
     <t>reproData</t>
   </si>
   <si>
-    <t>percR1 – percR15</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">estimated percent herbivory on the haphazardly selected reproductive unit (flower, fruit, seed) of the number corresponding to the column name. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note the protocol calls for up to 30 reproductive units so please add those columns if you sample more than 15</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t>ID number for plant within survey. Note</t>
     </r>
@@ -773,50 +711,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">across the total structures examined, a count of the number with some type of herbivory damage (chewing, piercing, boring). </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note that you only need to do EITHER the number of herbivore damaged units OR the percent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (both are provided as columns but you only need record one)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">across the total structures examined, an estimate of total percent damaged with some type of herbivory (chewing, piercing, boring). </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note that you only need to do EITHER the percent of herbivore damaged units OR the number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (both are provided as columns but you only need record one)</t>
-    </r>
-  </si>
-  <si>
     <t>number of pathogen damaged reproductive structures</t>
   </si>
   <si>
@@ -839,18 +733,6 @@
   </si>
   <si>
     <t>budding, flowering, fruiting</t>
-  </si>
-  <si>
-    <t>percent of pathogen damaged reproductive structures</t>
-  </si>
-  <si>
-    <t>percent of reproductive structures damaged by chewing herbivores</t>
-  </si>
-  <si>
-    <t>percent of reproductive structures damaged by piercing/sucking herbivores</t>
-  </si>
-  <si>
-    <t>percent of reproductive structures with damage not attributable to any distinct group</t>
   </si>
   <si>
     <t>whether you surveyed herbivores as a count or via presence absence</t>
@@ -1088,9 +970,6 @@
     <t>"true total", "subsample"</t>
   </si>
   <si>
-    <t>if you stopped at numLeaves = 60 but there were more leaves (see primary protocol) put "subsample". If you counted 60 leaves and that is the true total put "true total"</t>
-  </si>
-  <si>
     <t>NNdist_cm</t>
   </si>
   <si>
@@ -1139,9 +1018,6 @@
   </si>
   <si>
     <t>life stage of plant: seedling, vegetative, budding, flowering, fruiting; abbreviate s, v, b, fl, fr. If needed, feel free to enter more than one stage separated by semicolons (;)</t>
-  </si>
-  <si>
-    <t>Out of the numLeaves total, what is the number of leaves with herbivory (&gt; 0% damage)</t>
   </si>
   <si>
     <t>Remember that you are welcome to add more columns to the right of this one if you encounter insects without a pre-determined column. Define the columns in the "newColumns" sheet if you add any</t>
@@ -1378,6 +1254,81 @@
   </si>
   <si>
     <t>e.g., major</t>
+  </si>
+  <si>
+    <t>subsample_or_allRepro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of leaves on plant individual (including damaged leaves). If plant individual has ~60 leaves or less, count all leaves. If plant individual has more than ~ 60 leaves, record an estimated total count for the entire plant.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of reproductive structures on plant individual (including damaged structures). If plant individual has ~60 structures or less, count all structures. If plant individual has more than ~ 60 structures, record an estimated total count for the entire plant.  </t>
+  </si>
+  <si>
+    <t>If numRepro &gt; 60 and you plan to count damage on a subsample of 60 structures, put "subsample". If you will count damage on all structures (total in numRepro) put "true total"</t>
+  </si>
+  <si>
+    <t>If numLeaves &gt; 60 and you plan to count damage on a subsample of 60 leaves, put "subsample". If you will count damage on all leaves (total in numLeaves) put "true total"</t>
+  </si>
+  <si>
+    <t>b, fl, infl, imfr, mfr, infr, s</t>
+  </si>
+  <si>
+    <t>type of reproductive structure: flower buds (b), flowers (fl), inflorescences (infl), immature fruits (imfr), mature fruits (mfr), infructescenses (infr), or seeds (s)</t>
+  </si>
+  <si>
+    <t>numReproInv</t>
+  </si>
+  <si>
+    <t>Out of the numRepro total (or a subsample of 60, if you recorded "subsample" above), what is the number of structures that are inviable (i.e. completely destroyed such that they are not likely to produce viable seeds)</t>
+  </si>
+  <si>
+    <t>percReproHerbPlant</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">estimated percent herbivory on reproductive structures across the whole plant (visually estimated). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>If not feasible, can leave this blank.</t>
+    </r>
+  </si>
+  <si>
+    <t>percR1 – percR10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">estimated percent herbivory on the haphazardly selected reproductive unit (e.g. flower, fruit, seed) of the number corresponding to the column name. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Note the protocol calls for up to 10 reproductive units so please add those columns if you sample more than 10  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <t>Out of the numLeaves total (or out of 60, if you recorded "subsample" above), what is the number of leaves with herbivory (&gt; 0% damage)</t>
+  </si>
+  <si>
+    <t>Out of the numRepro total (or out of 60, if you recorded "subsample" above), what is the number of structures with herbivory (&gt; 0% damage)</t>
   </si>
 </sst>
 </file>
@@ -1549,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1691,9 +1642,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1829,9 +1777,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1881,6 +1826,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2203,9 +2178,9 @@
   </sheetPr>
   <dimension ref="A1:BZ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2307,27 +2282,27 @@
     </row>
     <row r="2" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
@@ -2335,31 +2310,31 @@
     </row>
     <row r="5" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -2368,11 +2343,11 @@
       <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="102"/>
+      <c r="E7" s="100"/>
     </row>
     <row r="8" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
@@ -2381,11 +2356,11 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="102"/>
+      <c r="E8" s="100"/>
     </row>
     <row r="9" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
@@ -2394,11 +2369,11 @@
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="102"/>
+      <c r="E9" s="100"/>
     </row>
     <row r="10" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -2407,46 +2382,46 @@
       <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="102"/>
+      <c r="E10" s="100"/>
     </row>
     <row r="11" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" s="102"/>
+        <v>202</v>
+      </c>
+      <c r="E11" s="100"/>
     </row>
     <row r="12" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="102"/>
+        <v>99</v>
+      </c>
+      <c r="E12" s="100"/>
     </row>
     <row r="13" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="102"/>
+        <v>91</v>
+      </c>
+      <c r="E13" s="100"/>
     </row>
     <row r="14" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B14" s="5" t="e">
         <f>densityData!D2</f>
@@ -2456,13 +2431,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E14" s="102"/>
+        <v>201</v>
+      </c>
+      <c r="E14" s="100"/>
     </row>
     <row r="15" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
@@ -2471,11 +2446,11 @@
       <c r="D15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="102"/>
+      <c r="E15" s="100"/>
     </row>
     <row r="16" spans="1:78" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -2484,11 +2459,11 @@
       <c r="D16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="102"/>
+      <c r="E16" s="100"/>
     </row>
     <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -2497,45 +2472,45 @@
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="102"/>
+      <c r="E17" s="100"/>
     </row>
     <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="102"/>
+      <c r="E18" s="100"/>
     </row>
     <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="102"/>
+        <v>97</v>
+      </c>
+      <c r="E19" s="100"/>
     </row>
     <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="17"/>
-      <c r="E20" s="102"/>
+      <c r="E20" s="100"/>
     </row>
     <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="102"/>
+      <c r="E21" s="100"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
@@ -2543,18 +2518,18 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="101" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" s="99" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A23" s="27" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2571,533 +2546,533 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AT103"/>
+  <dimension ref="A1:AT101"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="100"/>
-    <col min="2" max="2" width="32.5" style="54" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="83" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" style="83" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="63"/>
+    <col min="1" max="1" width="14.5" style="98"/>
+    <col min="2" max="2" width="32.5" style="53" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="82" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" style="82" customWidth="1"/>
+    <col min="5" max="16384" width="14.5" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="61" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" s="60" t="s">
+    <row r="1" spans="1:4" s="60" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="60" t="s">
-        <v>111</v>
+      <c r="D1" s="59" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="62" t="s">
-        <v>60</v>
+      <c r="A2" s="61" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A6" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C7" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A11" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="57" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="65" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="57" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A6" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="41" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="36" t="s">
+      <c r="C13" s="68"/>
+      <c r="D13" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="69" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="41" t="s">
+      <c r="D14" s="69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A16" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A17" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" s="78" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="74"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="77"/>
+      <c r="R20" s="77"/>
+      <c r="S20" s="77"/>
+      <c r="T20" s="77"/>
+      <c r="U20" s="77"/>
+      <c r="V20" s="77"/>
+      <c r="W20" s="77"/>
+      <c r="X20" s="77"/>
+      <c r="Y20" s="77"/>
+      <c r="Z20" s="77"/>
+      <c r="AA20" s="77"/>
+      <c r="AB20" s="77"/>
+    </row>
+    <row r="21" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A21" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="79" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="80" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="79" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" s="65" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A24" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C24" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="70" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A11" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="71" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A15" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="72" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A16" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="73" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A17" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:46" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="73" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:46" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="71" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:46" s="79" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="75"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="78"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="78"/>
-      <c r="Q20" s="78"/>
-      <c r="R20" s="78"/>
-      <c r="S20" s="78"/>
-      <c r="T20" s="78"/>
-      <c r="U20" s="78"/>
-      <c r="V20" s="78"/>
-      <c r="W20" s="78"/>
-      <c r="X20" s="78"/>
-      <c r="Y20" s="78"/>
-      <c r="Z20" s="78"/>
-      <c r="AA20" s="78"/>
-      <c r="AB20" s="78"/>
-    </row>
-    <row r="21" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A21" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="80" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:46" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="64" t="s">
-        <v>221</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="81" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="81" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:46" ht="14" x14ac:dyDescent="0.15">
-      <c r="A23" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="B23" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="80" t="s">
-        <v>216</v>
-      </c>
-      <c r="D23" s="80" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="24" spans="1:46" s="66" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A24" s="64" t="s">
-        <v>221</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="82" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="81" t="s">
-        <v>220</v>
+      <c r="D24" s="80" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A25" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="B25" s="54" t="s">
+      <c r="A25" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:46" s="79" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="84"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="86"/>
+      <c r="D25" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" s="78" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="83"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
     </row>
     <row r="27" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A27" s="62" t="s">
-        <v>62</v>
+      <c r="A27" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B27" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="80" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A28" s="64" t="s">
+      <c r="C27" s="67" t="s">
         <v>62</v>
       </c>
+      <c r="D27" s="79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A28" s="63" t="s">
+        <v>61</v>
+      </c>
       <c r="B28" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A29" s="61" t="s">
         <v>61</v>
-      </c>
-      <c r="D28" s="65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A29" s="62" t="s">
-        <v>62</v>
       </c>
       <c r="B29" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="80" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A30" s="64" t="s">
-        <v>62</v>
+      <c r="C29" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A30" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B30" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="81" t="s">
-        <v>177</v>
+      <c r="C30" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="80" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:46" ht="14" x14ac:dyDescent="0.15">
-      <c r="A31" s="62" t="s">
-        <v>62</v>
+      <c r="A31" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="68" t="s">
+      <c r="D31" s="67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A32" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A32" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="67" t="s">
-        <v>66</v>
-      </c>
       <c r="AT32" s="36"/>
     </row>
     <row r="33" spans="1:46" ht="14" x14ac:dyDescent="0.15">
-      <c r="A33" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="55" t="s">
+      <c r="A33" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="68" t="s">
+      <c r="C33" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="67" t="s">
         <v>70</v>
-      </c>
-      <c r="D33" s="68" t="s">
-        <v>71</v>
       </c>
       <c r="AS33" s="41"/>
       <c r="AT33" s="41"/>
     </row>
-    <row r="34" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A34" s="64" t="s">
-        <v>62</v>
+    <row r="34" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A34" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="67" t="s">
-        <v>79</v>
+        <v>207</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>77</v>
       </c>
       <c r="AR34" s="36"/>
       <c r="AS34" s="36"/>
       <c r="AT34" s="36"/>
     </row>
     <row r="35" spans="1:46" ht="70" x14ac:dyDescent="0.15">
-      <c r="A35" s="62" t="s">
-        <v>62</v>
+      <c r="A35" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B35" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="57" t="s">
-        <v>232</v>
+      <c r="C35" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="56" t="s">
+        <v>208</v>
       </c>
       <c r="AQ35" s="41"/>
       <c r="AR35" s="41"/>
       <c r="AS35" s="41"/>
       <c r="AT35" s="41"/>
     </row>
-    <row r="36" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A36" s="64" t="s">
-        <v>62</v>
+    <row r="36" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A36" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B36" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="67" t="s">
+      <c r="C36" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="86" t="s">
         <v>67</v>
-      </c>
-      <c r="D36" s="87" t="s">
-        <v>68</v>
       </c>
       <c r="AP36" s="36"/>
       <c r="AQ36" s="36"/>
@@ -3106,17 +3081,17 @@
       <c r="AT36" s="36"/>
     </row>
     <row r="37" spans="1:46" ht="14" x14ac:dyDescent="0.15">
-      <c r="A37" s="62" t="s">
-        <v>62</v>
+      <c r="A37" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="57" t="s">
-        <v>233</v>
+      <c r="C37" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="56" t="s">
+        <v>209</v>
       </c>
       <c r="AO37" s="41"/>
       <c r="AP37" s="41"/>
@@ -3125,18 +3100,18 @@
       <c r="AS37" s="41"/>
       <c r="AT37" s="41"/>
     </row>
-    <row r="38" spans="1:46" s="66" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A38" s="64" t="s">
-        <v>62</v>
+    <row r="38" spans="1:46" s="65" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A38" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B38" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="65" t="s">
-        <v>234</v>
+      <c r="C38" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>210</v>
       </c>
       <c r="AN38" s="36"/>
       <c r="AO38" s="36"/>
@@ -3147,17 +3122,17 @@
       <c r="AT38" s="36"/>
     </row>
     <row r="39" spans="1:46" ht="42" x14ac:dyDescent="0.15">
-      <c r="A39" s="62" t="s">
-        <v>62</v>
+      <c r="A39" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B39" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="57" t="s">
-        <v>178</v>
+      <c r="C39" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="56" t="s">
+        <v>163</v>
       </c>
       <c r="AM39" s="41"/>
       <c r="AN39" s="41"/>
@@ -3168,18 +3143,18 @@
       <c r="AS39" s="41"/>
       <c r="AT39" s="41"/>
     </row>
-    <row r="40" spans="1:46" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A40" s="64" t="s">
-        <v>62</v>
+    <row r="40" spans="1:46" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A40" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B40" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="67" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="67" t="s">
-        <v>74</v>
+      <c r="C40" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="66" t="s">
+        <v>73</v>
       </c>
       <c r="AL40" s="36"/>
       <c r="AM40" s="36"/>
@@ -3192,17 +3167,17 @@
       <c r="AT40" s="36"/>
     </row>
     <row r="41" spans="1:46" ht="14" x14ac:dyDescent="0.15">
-      <c r="A41" s="62" t="s">
-        <v>62</v>
+      <c r="A41" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="67" t="s">
         <v>75</v>
-      </c>
-      <c r="D41" s="68" t="s">
-        <v>76</v>
       </c>
       <c r="AK41" s="41"/>
       <c r="AL41" s="41"/>
@@ -3215,18 +3190,18 @@
       <c r="AS41" s="41"/>
       <c r="AT41" s="41"/>
     </row>
-    <row r="42" spans="1:46" s="66" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A42" s="64" t="s">
-        <v>62</v>
+    <row r="42" spans="1:46" s="65" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A42" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B42" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="67" t="s">
-        <v>77</v>
+      <c r="C42" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="70" t="s">
+        <v>231</v>
       </c>
       <c r="AJ42" s="36"/>
       <c r="AK42" s="36"/>
@@ -3241,17 +3216,17 @@
       <c r="AT42" s="36"/>
     </row>
     <row r="43" spans="1:46" ht="42" x14ac:dyDescent="0.15">
-      <c r="A43" s="62" t="s">
-        <v>62</v>
+      <c r="A43" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="C43" s="88" t="s">
-        <v>229</v>
-      </c>
-      <c r="D43" s="80" t="s">
-        <v>230</v>
+        <v>205</v>
+      </c>
+      <c r="C43" s="109" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="108" t="s">
+        <v>234</v>
       </c>
       <c r="AI43" s="41"/>
       <c r="AJ43" s="41"/>
@@ -3266,18 +3241,18 @@
       <c r="AS43" s="41"/>
       <c r="AT43" s="41"/>
     </row>
-    <row r="44" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A44" s="64" t="s">
-        <v>62</v>
+    <row r="44" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A44" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B44" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="65" t="s">
-        <v>235</v>
+      <c r="C44" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="70" t="s">
+        <v>243</v>
       </c>
       <c r="AH44" s="36"/>
       <c r="AI44" s="36"/>
@@ -3294,17 +3269,17 @@
       <c r="AT44" s="36"/>
     </row>
     <row r="45" spans="1:46" ht="42" x14ac:dyDescent="0.15">
-      <c r="A45" s="62" t="s">
-        <v>62</v>
+      <c r="A45" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="57" t="s">
-        <v>183</v>
+      <c r="C45" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="56" t="s">
+        <v>168</v>
       </c>
       <c r="AG45" s="41"/>
       <c r="AH45" s="41"/>
@@ -3321,18 +3296,18 @@
       <c r="AS45" s="41"/>
       <c r="AT45" s="41"/>
     </row>
-    <row r="46" spans="1:46" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A46" s="64" t="s">
-        <v>62</v>
+    <row r="46" spans="1:46" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A46" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B46" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="81" t="s">
-        <v>182</v>
+        <v>117</v>
+      </c>
+      <c r="C46" s="88" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="80" t="s">
+        <v>167</v>
       </c>
       <c r="AF46" s="36"/>
       <c r="AG46" s="36"/>
@@ -3350,17 +3325,17 @@
       <c r="AS46" s="36"/>
     </row>
     <row r="47" spans="1:46" ht="42" x14ac:dyDescent="0.15">
-      <c r="A47" s="62" t="s">
-        <v>62</v>
+      <c r="A47" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C47" s="80" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" s="80" t="s">
-        <v>181</v>
+        <v>118</v>
+      </c>
+      <c r="C47" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="79" t="s">
+        <v>166</v>
       </c>
       <c r="AE47" s="41"/>
       <c r="AF47" s="41"/>
@@ -3379,18 +3354,18 @@
       <c r="AS47" s="41"/>
       <c r="AT47" s="41"/>
     </row>
-    <row r="48" spans="1:46" s="66" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A48" s="64" t="s">
-        <v>62</v>
+    <row r="48" spans="1:46" s="65" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A48" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B48" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="C48" s="89" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" s="81" t="s">
-        <v>246</v>
+        <v>119</v>
+      </c>
+      <c r="C48" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="80" t="s">
+        <v>221</v>
       </c>
       <c r="AD48" s="42"/>
       <c r="AE48" s="36"/>
@@ -3411,35 +3386,35 @@
       <c r="AT48" s="36"/>
     </row>
     <row r="49" spans="1:46" ht="56" x14ac:dyDescent="0.15">
-      <c r="A49" s="62" t="s">
-        <v>207</v>
+      <c r="A49" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="57" t="s">
-        <v>249</v>
+        <v>120</v>
+      </c>
+      <c r="C49" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="56" t="s">
+        <v>224</v>
       </c>
       <c r="P49" s="40"/>
       <c r="Q49" s="40"/>
       <c r="R49" s="40"/>
       <c r="S49" s="39"/>
     </row>
-    <row r="50" spans="1:46" s="66" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A50" s="64" t="s">
-        <v>207</v>
+    <row r="50" spans="1:46" s="65" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A50" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B50" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C50" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="D50" s="65" t="s">
-        <v>250</v>
+        <v>121</v>
+      </c>
+      <c r="C50" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="64" t="s">
+        <v>225</v>
       </c>
       <c r="O50" s="43"/>
       <c r="P50" s="43"/>
@@ -3448,17 +3423,17 @@
       <c r="S50" s="42"/>
     </row>
     <row r="51" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A51" s="62" t="s">
-        <v>62</v>
+      <c r="A51" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="57" t="s">
-        <v>184</v>
+        <v>149</v>
+      </c>
+      <c r="C51" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="92" t="s">
+        <v>169</v>
       </c>
       <c r="U51" s="39"/>
       <c r="V51" s="39"/>
@@ -3479,18 +3454,18 @@
       <c r="AK51" s="41"/>
       <c r="AL51" s="41"/>
     </row>
-    <row r="52" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A52" s="64" t="s">
-        <v>62</v>
+    <row r="52" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A52" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="B52" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" s="65" t="s">
-        <v>185</v>
+      <c r="C52" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="64" t="s">
+        <v>170</v>
       </c>
       <c r="E52" s="43"/>
       <c r="F52" s="42"/>
@@ -3536,17 +3511,17 @@
       <c r="AT52" s="36"/>
     </row>
     <row r="53" spans="1:46" ht="56" x14ac:dyDescent="0.15">
-      <c r="A53" s="62" t="s">
-        <v>62</v>
+      <c r="A53" s="61" t="s">
+        <v>61</v>
       </c>
       <c r="B53" s="41" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D53" s="57" t="s">
-        <v>186</v>
+        <v>154</v>
+      </c>
+      <c r="C53" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="56" t="s">
+        <v>171</v>
       </c>
       <c r="E53" s="41"/>
       <c r="F53" s="41"/>
@@ -3591,442 +3566,457 @@
       <c r="AS53" s="41"/>
       <c r="AT53" s="41"/>
     </row>
-    <row r="54" spans="1:46" s="79" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="84"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="49"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="49"/>
-      <c r="O54" s="49"/>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="49"/>
-      <c r="R54" s="52"/>
-      <c r="S54" s="52"/>
-      <c r="T54" s="53"/>
-      <c r="U54" s="53"/>
-      <c r="V54" s="53"/>
-      <c r="W54" s="53"/>
-      <c r="X54" s="53"/>
-      <c r="Y54" s="53"/>
-      <c r="Z54" s="53"/>
-      <c r="AA54" s="53"/>
-      <c r="AB54" s="53"/>
-      <c r="AC54" s="53"/>
-      <c r="AD54" s="53"/>
-      <c r="AE54" s="49"/>
-      <c r="AF54" s="49"/>
-      <c r="AG54" s="49"/>
-      <c r="AH54" s="49"/>
-      <c r="AI54" s="49"/>
-      <c r="AJ54" s="49"/>
-      <c r="AK54" s="49"/>
-      <c r="AL54" s="49"/>
-      <c r="AM54" s="49"/>
-      <c r="AN54" s="49"/>
-      <c r="AO54" s="49"/>
-      <c r="AP54" s="49"/>
-      <c r="AQ54" s="49"/>
-      <c r="AR54" s="49"/>
-      <c r="AS54" s="49"/>
-      <c r="AT54" s="49"/>
+    <row r="54" spans="1:46" s="78" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A54" s="83"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="48"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="48"/>
+      <c r="P54" s="48"/>
+      <c r="Q54" s="48"/>
+      <c r="R54" s="51"/>
+      <c r="S54" s="51"/>
+      <c r="T54" s="52"/>
+      <c r="U54" s="52"/>
+      <c r="V54" s="52"/>
+      <c r="W54" s="52"/>
+      <c r="X54" s="52"/>
+      <c r="Y54" s="52"/>
+      <c r="Z54" s="52"/>
+      <c r="AA54" s="52"/>
+      <c r="AB54" s="52"/>
+      <c r="AC54" s="52"/>
+      <c r="AD54" s="52"/>
+      <c r="AE54" s="48"/>
+      <c r="AF54" s="48"/>
+      <c r="AG54" s="48"/>
+      <c r="AH54" s="48"/>
+      <c r="AI54" s="48"/>
+      <c r="AJ54" s="48"/>
+      <c r="AK54" s="48"/>
+      <c r="AL54" s="48"/>
+      <c r="AM54" s="48"/>
+      <c r="AN54" s="48"/>
+      <c r="AO54" s="48"/>
+      <c r="AP54" s="48"/>
+      <c r="AQ54" s="48"/>
+      <c r="AR54" s="48"/>
+      <c r="AS54" s="48"/>
+      <c r="AT54" s="48"/>
     </row>
     <row r="55" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A55" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B55" s="90" t="s">
+      <c r="A55" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="68" t="s">
+      <c r="C55" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A56" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56" s="64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A57" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="80" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="56" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A56" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A57" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B57" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" s="80" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" spans="1:46" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A58" s="64" t="s">
-        <v>188</v>
+      <c r="D57" s="79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:46" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A58" s="63" t="s">
+        <v>173</v>
       </c>
       <c r="B58" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="67" t="s">
+      <c r="C58" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="80" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A59" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:46" s="65" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A60" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="D60" s="70" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="1:46" ht="28" x14ac:dyDescent="0.15">
+      <c r="A61" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="91" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="87" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:46" s="65" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A62" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="80" t="s">
+        <v>179</v>
+      </c>
+      <c r="D62" s="80" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:46" ht="56" x14ac:dyDescent="0.15">
+      <c r="A63" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="92" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="64" spans="1:46" s="65" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A64" s="112" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" s="88" t="s">
+        <v>206</v>
+      </c>
+      <c r="D64" s="113" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A65" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="C65" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="92" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" s="65" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A66" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="110" t="s">
+        <v>237</v>
+      </c>
+      <c r="C66" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66" s="70" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" ht="14" x14ac:dyDescent="0.15">
+      <c r="A67" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="79" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A68" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="80" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A69" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B69" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="79" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A70" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="80" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A71" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="111" t="s">
+        <v>239</v>
+      </c>
+      <c r="C71" s="92" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="92" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" s="65" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A72" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="110" t="s">
+        <v>241</v>
+      </c>
+      <c r="C72" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="70" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A73" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" s="78" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A74" s="83"/>
+      <c r="B74" s="93"/>
+      <c r="C74" s="94"/>
+      <c r="D74" s="50"/>
+    </row>
+    <row r="75" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A75" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B75" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" s="79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A76" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A77" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="81" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A59" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B59" s="90" t="s">
+      <c r="D77" s="79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A78" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="R78" s="43"/>
+      <c r="S78" s="42"/>
+    </row>
+    <row r="79" spans="1:19" ht="28" x14ac:dyDescent="0.15">
+      <c r="A79" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B79" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59" s="57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="60" spans="1:46" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A60" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B60" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="71" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A61" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B61" s="92" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="57" t="s">
-        <v>201</v>
-      </c>
-      <c r="D61" s="88" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="62" spans="1:46" s="66" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A62" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B62" s="91" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="81" t="s">
-        <v>198</v>
-      </c>
-      <c r="D62" s="81" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="63" spans="1:46" ht="28" x14ac:dyDescent="0.15">
-      <c r="A63" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B63" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="93" t="s">
+      <c r="C79" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="93" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="64" spans="1:46" s="66" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A64" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B64" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" s="65" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" ht="14" x14ac:dyDescent="0.15">
-      <c r="A65" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B65" s="90" t="s">
-        <v>123</v>
-      </c>
-      <c r="C65" s="93" t="s">
-        <v>69</v>
-      </c>
-      <c r="D65" s="80" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A66" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B66" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C66" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" s="81" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A67" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B67" s="90" t="s">
+      <c r="D79" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q79" s="40"/>
+      <c r="R79" s="40"/>
+      <c r="S79" s="39"/>
+    </row>
+    <row r="80" spans="1:19" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A80" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="B80" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="93" t="s">
-        <v>69</v>
-      </c>
-      <c r="D67" s="80" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A68" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B68" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="C68" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="81" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" ht="70" x14ac:dyDescent="0.15">
-      <c r="A69" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B69" s="92" t="s">
-        <v>47</v>
-      </c>
-      <c r="C69" s="93" t="s">
-        <v>67</v>
-      </c>
-      <c r="D69" s="57" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A70" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B70" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" s="89" t="s">
-        <v>67</v>
-      </c>
-      <c r="D70" s="81" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" ht="14" x14ac:dyDescent="0.15">
-      <c r="A71" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B71" s="90" t="s">
-        <v>135</v>
-      </c>
-      <c r="C71" s="88" t="s">
-        <v>67</v>
-      </c>
-      <c r="D71" s="80" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A72" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B72" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" s="89" t="s">
-        <v>67</v>
-      </c>
-      <c r="D72" s="81" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A73" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B73" s="90" t="s">
-        <v>137</v>
-      </c>
-      <c r="C73" s="94" t="s">
-        <v>67</v>
-      </c>
-      <c r="D73" s="80" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" s="66" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A74" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B74" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="C74" s="89" t="s">
-        <v>67</v>
-      </c>
-      <c r="D74" s="65" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A75" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="B75" s="90" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" s="57" t="s">
+      <c r="C80" s="95" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" s="79" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="84"/>
-      <c r="B76" s="95"/>
-      <c r="C76" s="96"/>
-      <c r="D76" s="51"/>
-    </row>
-    <row r="77" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A77" s="62" t="s">
-        <v>207</v>
-      </c>
-      <c r="B77" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C77" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="D77" s="80" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A78" s="64" t="s">
-        <v>207</v>
-      </c>
-      <c r="B78" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C78" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="D78" s="65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="A79" s="62" t="s">
-        <v>207</v>
-      </c>
-      <c r="B79" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C79" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D79" s="80" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A80" s="64" t="s">
-        <v>207</v>
-      </c>
-      <c r="B80" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="D80" s="81" t="s">
-        <v>177</v>
-      </c>
+      <c r="D80" s="96" t="s">
+        <v>183</v>
+      </c>
+      <c r="N80" s="43"/>
+      <c r="O80" s="43"/>
+      <c r="P80" s="43"/>
+      <c r="Q80" s="43"/>
       <c r="R80" s="43"/>
       <c r="S80" s="42"/>
     </row>
     <row r="81" spans="1:28" ht="28" x14ac:dyDescent="0.15">
-      <c r="A81" s="62" t="s">
-        <v>207</v>
+      <c r="A81" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C81" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D81" s="57" t="s">
-        <v>191</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C81" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="M81" s="40"/>
+      <c r="N81" s="40"/>
+      <c r="O81" s="40"/>
+      <c r="P81" s="40"/>
       <c r="Q81" s="40"/>
       <c r="R81" s="40"/>
       <c r="S81" s="39"/>
     </row>
-    <row r="82" spans="1:28" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A82" s="64" t="s">
-        <v>207</v>
+    <row r="82" spans="1:28" s="65" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A82" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B82" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="C82" s="97" t="s">
-        <v>208</v>
-      </c>
-      <c r="D82" s="98" t="s">
-        <v>206</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C82" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D82" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="L82" s="42"/>
+      <c r="M82" s="43"/>
       <c r="N82" s="43"/>
       <c r="O82" s="43"/>
       <c r="P82" s="43"/>
@@ -4034,19 +4024,21 @@
       <c r="R82" s="43"/>
       <c r="S82" s="42"/>
     </row>
-    <row r="83" spans="1:28" ht="28" x14ac:dyDescent="0.15">
-      <c r="A83" s="62" t="s">
-        <v>207</v>
+    <row r="83" spans="1:28" ht="70" x14ac:dyDescent="0.15">
+      <c r="A83" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C83" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D83" s="57" t="s">
-        <v>211</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C83" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D83" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="K83" s="39"/>
+      <c r="L83" s="39"/>
       <c r="M83" s="40"/>
       <c r="N83" s="40"/>
       <c r="O83" s="40"/>
@@ -4055,19 +4047,20 @@
       <c r="R83" s="40"/>
       <c r="S83" s="39"/>
     </row>
-    <row r="84" spans="1:28" s="66" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A84" s="64" t="s">
-        <v>207</v>
+    <row r="84" spans="1:28" s="65" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A84" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B84" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C84" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="D84" s="65" t="s">
-        <v>245</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C84" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D84" s="64" t="s">
+        <v>216</v>
+      </c>
+      <c r="K84" s="42"/>
       <c r="L84" s="42"/>
       <c r="M84" s="43"/>
       <c r="N84" s="43"/>
@@ -4077,157 +4070,187 @@
       <c r="R84" s="43"/>
       <c r="S84" s="42"/>
     </row>
-    <row r="85" spans="1:28" ht="70" x14ac:dyDescent="0.15">
-      <c r="A85" s="62" t="s">
-        <v>207</v>
+    <row r="85" spans="1:28" ht="56" x14ac:dyDescent="0.15">
+      <c r="A85" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B85" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C85" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D85" s="57" t="s">
-        <v>240</v>
-      </c>
-      <c r="K85" s="39"/>
-      <c r="L85" s="39"/>
-      <c r="M85" s="40"/>
-      <c r="N85" s="40"/>
-      <c r="O85" s="40"/>
-      <c r="P85" s="40"/>
-      <c r="Q85" s="40"/>
-      <c r="R85" s="40"/>
-      <c r="S85" s="39"/>
-    </row>
-    <row r="86" spans="1:28" s="66" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A86" s="64" t="s">
-        <v>207</v>
+        <v>43</v>
+      </c>
+      <c r="C85" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D85" s="56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" s="65" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A86" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B86" s="43" t="s">
-        <v>237</v>
-      </c>
-      <c r="C86" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D86" s="65" t="s">
-        <v>241</v>
-      </c>
-      <c r="K86" s="42"/>
-      <c r="L86" s="42"/>
-      <c r="M86" s="43"/>
-      <c r="N86" s="43"/>
-      <c r="O86" s="43"/>
-      <c r="P86" s="43"/>
-      <c r="Q86" s="43"/>
-      <c r="R86" s="43"/>
-      <c r="S86" s="42"/>
+        <v>213</v>
+      </c>
+      <c r="C86" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D86" s="64" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="87" spans="1:28" ht="56" x14ac:dyDescent="0.15">
-      <c r="A87" s="62" t="s">
-        <v>207</v>
+      <c r="A87" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C87" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D87" s="57" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="88" spans="1:28" s="66" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A88" s="64" t="s">
-        <v>207</v>
+        <v>123</v>
+      </c>
+      <c r="C87" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" s="79" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A88" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>238</v>
-      </c>
-      <c r="C88" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="D88" s="65" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="89" spans="1:28" ht="56" x14ac:dyDescent="0.15">
-      <c r="A89" s="62" t="s">
-        <v>207</v>
+        <v>148</v>
+      </c>
+      <c r="C88" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D88" s="80" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" ht="28" x14ac:dyDescent="0.15">
+      <c r="A89" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="C89" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D89" s="80" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="90" spans="1:28" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A90" s="64" t="s">
-        <v>207</v>
+        <v>126</v>
+      </c>
+      <c r="C89" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D89" s="79" t="s">
+        <v>189</v>
+      </c>
+      <c r="F89" s="97"/>
+      <c r="G89" s="97"/>
+      <c r="H89" s="97"/>
+      <c r="I89" s="97"/>
+      <c r="J89" s="97"/>
+      <c r="K89" s="97"/>
+      <c r="L89" s="97"/>
+      <c r="M89" s="97"/>
+      <c r="N89" s="97"/>
+      <c r="O89" s="97"/>
+      <c r="P89" s="97"/>
+      <c r="Q89" s="97"/>
+      <c r="R89" s="97"/>
+      <c r="S89" s="97"/>
+      <c r="T89" s="97"/>
+      <c r="U89" s="97"/>
+      <c r="V89" s="97"/>
+      <c r="W89" s="97"/>
+      <c r="X89" s="97"/>
+      <c r="Y89" s="97"/>
+      <c r="Z89" s="97"/>
+      <c r="AA89" s="97"/>
+      <c r="AB89" s="97"/>
+    </row>
+    <row r="90" spans="1:28" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A90" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="C90" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="D90" s="81" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="91" spans="1:28" ht="28" x14ac:dyDescent="0.15">
-      <c r="A91" s="62" t="s">
-        <v>207</v>
+        <v>127</v>
+      </c>
+      <c r="C90" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D90" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+      <c r="I90" s="44"/>
+      <c r="J90" s="44"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="44"/>
+      <c r="M90" s="44"/>
+      <c r="N90" s="44"/>
+      <c r="O90" s="44"/>
+      <c r="P90" s="44"/>
+      <c r="Q90" s="44"/>
+      <c r="R90" s="44"/>
+      <c r="S90" s="44"/>
+      <c r="T90" s="44"/>
+      <c r="U90" s="44"/>
+      <c r="V90" s="44"/>
+      <c r="W90" s="44"/>
+      <c r="X90" s="44"/>
+      <c r="Y90" s="44"/>
+      <c r="Z90" s="44"/>
+      <c r="AA90" s="44"/>
+      <c r="AB90" s="44"/>
+    </row>
+    <row r="91" spans="1:28" ht="56" x14ac:dyDescent="0.15">
+      <c r="A91" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B91" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="C91" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D91" s="80" t="s">
-        <v>212</v>
-      </c>
-      <c r="F91" s="99"/>
-      <c r="G91" s="99"/>
-      <c r="H91" s="99"/>
-      <c r="I91" s="99"/>
-      <c r="J91" s="99"/>
-      <c r="K91" s="99"/>
-      <c r="L91" s="99"/>
-      <c r="M91" s="99"/>
-      <c r="N91" s="99"/>
-      <c r="O91" s="99"/>
-      <c r="P91" s="99"/>
-      <c r="Q91" s="99"/>
-      <c r="R91" s="99"/>
-      <c r="S91" s="99"/>
-      <c r="T91" s="99"/>
-      <c r="U91" s="99"/>
-      <c r="V91" s="99"/>
-      <c r="W91" s="99"/>
-      <c r="X91" s="99"/>
-      <c r="Y91" s="99"/>
-      <c r="Z91" s="99"/>
-      <c r="AA91" s="99"/>
-      <c r="AB91" s="99"/>
-    </row>
-    <row r="92" spans="1:28" s="66" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A92" s="64" t="s">
-        <v>207</v>
+        <v>226</v>
+      </c>
+      <c r="C91" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D91" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="E91" s="97"/>
+      <c r="F91" s="97"/>
+      <c r="G91" s="97"/>
+      <c r="H91" s="97"/>
+      <c r="I91" s="97"/>
+      <c r="J91" s="97"/>
+      <c r="K91" s="97"/>
+      <c r="L91" s="97"/>
+      <c r="M91" s="97"/>
+      <c r="N91" s="97"/>
+      <c r="O91" s="97"/>
+      <c r="P91" s="97"/>
+      <c r="Q91" s="97"/>
+      <c r="R91" s="97"/>
+      <c r="S91" s="97"/>
+      <c r="T91" s="97"/>
+      <c r="U91" s="97"/>
+      <c r="V91" s="97"/>
+      <c r="W91" s="97"/>
+      <c r="X91" s="97"/>
+      <c r="Y91" s="97"/>
+      <c r="Z91" s="97"/>
+      <c r="AA91" s="97"/>
+      <c r="AB91" s="97"/>
+    </row>
+    <row r="92" spans="1:28" s="65" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A92" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>141</v>
-      </c>
-      <c r="C92" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="D92" s="81" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="C92" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D92" s="80" t="s">
+        <v>219</v>
       </c>
       <c r="E92" s="44"/>
       <c r="F92" s="44"/>
@@ -4254,142 +4277,66 @@
       <c r="AA92" s="44"/>
       <c r="AB92" s="44"/>
     </row>
-    <row r="93" spans="1:28" ht="56" x14ac:dyDescent="0.15">
-      <c r="A93" s="62" t="s">
-        <v>207</v>
+    <row r="93" spans="1:28" ht="28" x14ac:dyDescent="0.15">
+      <c r="A93" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="C93" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D93" s="80" t="s">
-        <v>214</v>
-      </c>
-      <c r="E93" s="99"/>
-      <c r="F93" s="99"/>
-      <c r="G93" s="99"/>
-      <c r="H93" s="99"/>
-      <c r="I93" s="99"/>
-      <c r="J93" s="99"/>
-      <c r="K93" s="99"/>
-      <c r="L93" s="99"/>
-      <c r="M93" s="99"/>
-      <c r="N93" s="99"/>
-      <c r="O93" s="99"/>
-      <c r="P93" s="99"/>
-      <c r="Q93" s="99"/>
-      <c r="R93" s="99"/>
-      <c r="S93" s="99"/>
-      <c r="T93" s="99"/>
-      <c r="U93" s="99"/>
-      <c r="V93" s="99"/>
-      <c r="W93" s="99"/>
-      <c r="X93" s="99"/>
-      <c r="Y93" s="99"/>
-      <c r="Z93" s="99"/>
-      <c r="AA93" s="99"/>
-      <c r="AB93" s="99"/>
-    </row>
-    <row r="94" spans="1:28" s="66" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A94" s="64" t="s">
-        <v>207</v>
-      </c>
-      <c r="B94" s="43" t="s">
-        <v>239</v>
-      </c>
-      <c r="C94" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D94" s="81" t="s">
-        <v>244</v>
-      </c>
-      <c r="E94" s="44"/>
-      <c r="F94" s="44"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="44"/>
-      <c r="I94" s="44"/>
-      <c r="J94" s="44"/>
-      <c r="K94" s="44"/>
-      <c r="L94" s="44"/>
-      <c r="M94" s="44"/>
-      <c r="N94" s="44"/>
-      <c r="O94" s="44"/>
-      <c r="P94" s="44"/>
-      <c r="Q94" s="44"/>
-      <c r="R94" s="44"/>
-      <c r="S94" s="44"/>
-      <c r="T94" s="44"/>
-      <c r="U94" s="44"/>
-      <c r="V94" s="44"/>
-      <c r="W94" s="44"/>
-      <c r="X94" s="44"/>
-      <c r="Y94" s="44"/>
-      <c r="Z94" s="44"/>
-      <c r="AA94" s="44"/>
-      <c r="AB94" s="44"/>
+        <v>3</v>
+      </c>
+      <c r="C93" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="D93" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="E93" s="97"/>
+      <c r="F93" s="97"/>
+      <c r="G93" s="97"/>
+      <c r="H93" s="97"/>
+      <c r="I93" s="97"/>
+      <c r="J93" s="97"/>
+      <c r="K93" s="97"/>
+      <c r="L93" s="97"/>
+      <c r="M93" s="97"/>
+      <c r="N93" s="97"/>
+      <c r="O93" s="97"/>
+      <c r="P93" s="97"/>
+      <c r="Q93" s="97"/>
+      <c r="R93" s="97"/>
+      <c r="S93" s="97"/>
+      <c r="T93" s="97"/>
+      <c r="U93" s="97"/>
+      <c r="V93" s="97"/>
+      <c r="W93" s="97"/>
+      <c r="X93" s="97"/>
+      <c r="Y93" s="97"/>
+      <c r="Z93" s="97"/>
+      <c r="AA93" s="97"/>
+      <c r="AB93" s="97"/>
+    </row>
+    <row r="94" spans="1:28" s="78" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A94" s="74"/>
+      <c r="B94" s="75"/>
+      <c r="C94" s="76"/>
+      <c r="D94" s="76"/>
     </row>
     <row r="95" spans="1:28" ht="28" x14ac:dyDescent="0.15">
-      <c r="A95" s="62" t="s">
-        <v>207</v>
-      </c>
-      <c r="B95" s="40" t="s">
+      <c r="A95" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C95" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="D95" s="57" t="s">
-        <v>185</v>
-      </c>
-      <c r="E95" s="99"/>
-      <c r="F95" s="99"/>
-      <c r="G95" s="99"/>
-      <c r="H95" s="99"/>
-      <c r="I95" s="99"/>
-      <c r="J95" s="99"/>
-      <c r="K95" s="99"/>
-      <c r="L95" s="99"/>
-      <c r="M95" s="99"/>
-      <c r="N95" s="99"/>
-      <c r="O95" s="99"/>
-      <c r="P95" s="99"/>
-      <c r="Q95" s="99"/>
-      <c r="R95" s="99"/>
-      <c r="S95" s="99"/>
-      <c r="T95" s="99"/>
-      <c r="U95" s="99"/>
-      <c r="V95" s="99"/>
-      <c r="W95" s="99"/>
-      <c r="X95" s="99"/>
-      <c r="Y95" s="99"/>
-      <c r="Z95" s="99"/>
-      <c r="AA95" s="99"/>
-      <c r="AB95" s="99"/>
-    </row>
-    <row r="96" spans="1:28" s="79" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A96" s="75"/>
-      <c r="B96" s="76"/>
-      <c r="C96" s="77"/>
-      <c r="D96" s="77"/>
-    </row>
-    <row r="97" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A97" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="D97" s="80" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="102" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="103" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
+      <c r="B95" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D95" s="79" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vNDbI5uCRwfevhvgzhNSdXPfzShCQ+gCblMGpSJC9fa5zAYY/OVdaME1aYO2yxkMmKHW0VJEN+sHkbi8Q7fk9A==" saltValue="U/pmpopB3XZKXfRSPRJjbg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="sfqBxsPGCBs3fQ4fqUkLHMJmcvvucnYnd3RpBL/SB/uaZNQiJgJMOXgL/2pWU0yYHFG9yvkmbEFtUuGEz6kpXg==" saltValue="Vo+F/ZChAWeOA+BO4j0PfA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
@@ -4406,7 +4353,7 @@
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4421,16 +4368,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>3</v>
@@ -4450,7 +4397,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4459,7 +4406,7 @@
       </c>
       <c r="B3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4547,7 +4494,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4588,7 +4535,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" s="42" t="s">
         <v>11</v>
@@ -4597,16 +4544,16 @@
         <v>19</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="I1" s="43" t="s">
         <v>23</v>
@@ -4633,7 +4580,7 @@
         <v>28</v>
       </c>
       <c r="Q1" s="43" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="R1" s="42" t="s">
         <v>29</v>
@@ -4642,19 +4589,19 @@
         <v>30</v>
       </c>
       <c r="T1" s="43" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="U1" s="43" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="V1" s="43" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="W1" s="43" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="X1" s="43" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="Y1" s="42" t="s">
         <v>31</v>
@@ -4690,64 +4637,64 @@
         <v>3</v>
       </c>
       <c r="AJ1" s="43" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="AK1" s="43" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="AL1" s="43" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="AM1" s="43" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="AN1" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO1" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP1" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ1" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR1" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS1" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT1" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU1" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV1" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW1" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="AX1" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="AY1" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="AZ1" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="BA1" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="BB1" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="BC1" s="36" t="s">
         <v>146</v>
-      </c>
-      <c r="AO1" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP1" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="AQ1" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="AR1" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="AS1" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT1" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU1" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="AV1" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="AW1" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="AX1" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="AY1" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="AZ1" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="BA1" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="BB1" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="BC1" s="36" t="s">
-        <v>161</v>
       </c>
       <c r="BD1" s="24"/>
       <c r="BE1" s="23"/>
@@ -4767,23 +4714,23 @@
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
       <c r="G2" s="21"/>
-      <c r="H2" s="103"/>
+      <c r="H2" s="101"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="104" t="s">
-        <v>247</v>
-      </c>
-      <c r="N2" s="104" t="s">
-        <v>248</v>
-      </c>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="103"/>
+      <c r="M2" s="102" t="s">
+        <v>222</v>
+      </c>
+      <c r="N2" s="102" t="s">
+        <v>223</v>
+      </c>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="101"/>
       <c r="S2" s="28"/>
-      <c r="U2" s="106"/>
+      <c r="U2" s="104"/>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
       <c r="AA2" s="28"/>
@@ -4808,17 +4755,17 @@
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="21"/>
-      <c r="H3" s="103"/>
+      <c r="H3" s="101"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
       <c r="L3" s="28"/>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
       <c r="S3" s="28"/>
       <c r="Y3" s="28"/>
       <c r="Z3" s="28"/>
@@ -4844,17 +4791,17 @@
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="21"/>
-      <c r="H4" s="103"/>
+      <c r="H4" s="101"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
-      <c r="O4" s="103"/>
-      <c r="P4" s="103"/>
-      <c r="Q4" s="103"/>
-      <c r="R4" s="103"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
       <c r="S4" s="28"/>
       <c r="Y4" s="28"/>
       <c r="Z4" s="28"/>
@@ -4887,10 +4834,10 @@
       <c r="L5" s="28"/>
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
       <c r="S5" s="28"/>
       <c r="Y5" s="28"/>
       <c r="Z5" s="28"/>
@@ -4916,17 +4863,17 @@
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="103"/>
+      <c r="H6" s="101"/>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103"/>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="103"/>
+      <c r="O6" s="101"/>
+      <c r="P6" s="101"/>
+      <c r="Q6" s="101"/>
+      <c r="R6" s="101"/>
       <c r="S6" s="28"/>
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
@@ -4952,17 +4899,17 @@
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="103"/>
+      <c r="H7" s="101"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
-      <c r="O7" s="103"/>
-      <c r="P7" s="103"/>
-      <c r="Q7" s="103"/>
-      <c r="R7" s="103"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
       <c r="S7" s="28"/>
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
@@ -4988,17 +4935,17 @@
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="103"/>
+      <c r="H8" s="101"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="101"/>
       <c r="S8" s="28"/>
       <c r="Y8" s="28"/>
       <c r="Z8" s="28"/>
@@ -5024,17 +4971,17 @@
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="103"/>
+      <c r="H9" s="101"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103"/>
-      <c r="Q9" s="103"/>
-      <c r="R9" s="103"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
       <c r="S9" s="28"/>
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
@@ -5060,17 +5007,17 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="21"/>
-      <c r="H10" s="103"/>
+      <c r="H10" s="101"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
-      <c r="O10" s="103"/>
-      <c r="P10" s="103"/>
-      <c r="Q10" s="103"/>
-      <c r="R10" s="103"/>
+      <c r="O10" s="101"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
+      <c r="R10" s="101"/>
       <c r="S10" s="28"/>
       <c r="Y10" s="28"/>
       <c r="Z10" s="28"/>
@@ -5096,17 +5043,17 @@
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="103"/>
+      <c r="H11" s="101"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
+      <c r="O11" s="101"/>
+      <c r="P11" s="101"/>
+      <c r="Q11" s="101"/>
+      <c r="R11" s="101"/>
       <c r="S11" s="28"/>
       <c r="Y11" s="28"/>
       <c r="Z11" s="28"/>
@@ -5132,17 +5079,17 @@
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="103"/>
+      <c r="H12" s="101"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="103"/>
-      <c r="P12" s="103"/>
-      <c r="Q12" s="103"/>
-      <c r="R12" s="103"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
       <c r="S12" s="28"/>
       <c r="Y12" s="28"/>
       <c r="Z12" s="28"/>
@@ -5168,17 +5115,17 @@
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="103"/>
+      <c r="H13" s="101"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="101"/>
       <c r="S13" s="28"/>
       <c r="Y13" s="28"/>
       <c r="Z13" s="28"/>
@@ -5204,17 +5151,17 @@
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="103"/>
+      <c r="H14" s="101"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
+      <c r="O14" s="101"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="101"/>
+      <c r="R14" s="101"/>
       <c r="S14" s="28"/>
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
@@ -5240,17 +5187,17 @@
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="103"/>
+      <c r="H15" s="101"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
-      <c r="O15" s="103"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
+      <c r="O15" s="101"/>
+      <c r="P15" s="101"/>
+      <c r="Q15" s="101"/>
+      <c r="R15" s="101"/>
       <c r="S15" s="28"/>
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
@@ -5276,17 +5223,17 @@
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="103"/>
+      <c r="H16" s="101"/>
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
+      <c r="O16" s="101"/>
+      <c r="P16" s="101"/>
+      <c r="Q16" s="101"/>
+      <c r="R16" s="101"/>
       <c r="S16" s="28"/>
       <c r="Y16" s="28"/>
       <c r="Z16" s="28"/>
@@ -5312,17 +5259,17 @@
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="103"/>
+      <c r="H17" s="101"/>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="103"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
+      <c r="O17" s="101"/>
+      <c r="P17" s="101"/>
+      <c r="Q17" s="101"/>
+      <c r="R17" s="101"/>
       <c r="S17" s="28"/>
       <c r="Y17" s="28"/>
       <c r="Z17" s="28"/>
@@ -5348,17 +5295,17 @@
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="103"/>
+      <c r="H18" s="101"/>
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
+      <c r="O18" s="101"/>
+      <c r="P18" s="101"/>
+      <c r="Q18" s="101"/>
+      <c r="R18" s="101"/>
       <c r="S18" s="28"/>
       <c r="Y18" s="28"/>
       <c r="Z18" s="28"/>
@@ -5384,17 +5331,17 @@
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="103"/>
+      <c r="H19" s="101"/>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="103"/>
-      <c r="R19" s="103"/>
+      <c r="O19" s="101"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="101"/>
+      <c r="R19" s="101"/>
       <c r="S19" s="28"/>
       <c r="Y19" s="28"/>
       <c r="Z19" s="28"/>
@@ -5420,17 +5367,17 @@
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="103"/>
+      <c r="H20" s="101"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
+      <c r="O20" s="101"/>
+      <c r="P20" s="101"/>
+      <c r="Q20" s="101"/>
+      <c r="R20" s="101"/>
       <c r="S20" s="28"/>
       <c r="Y20" s="28"/>
       <c r="Z20" s="28"/>
@@ -5456,17 +5403,17 @@
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="103"/>
+      <c r="H21" s="101"/>
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
-      <c r="O21" s="103"/>
-      <c r="P21" s="103"/>
-      <c r="Q21" s="103"/>
-      <c r="R21" s="103"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="101"/>
+      <c r="Q21" s="101"/>
+      <c r="R21" s="101"/>
       <c r="S21" s="28"/>
       <c r="Y21" s="28"/>
       <c r="Z21" s="28"/>
@@ -5492,17 +5439,17 @@
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
-      <c r="O22" s="103"/>
-      <c r="P22" s="103"/>
-      <c r="Q22" s="103"/>
-      <c r="R22" s="103"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="101"/>
+      <c r="Q22" s="101"/>
+      <c r="R22" s="101"/>
       <c r="S22" s="28"/>
       <c r="Y22" s="28"/>
       <c r="Z22" s="28"/>
@@ -5528,17 +5475,17 @@
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="103"/>
+      <c r="H23" s="101"/>
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="103"/>
-      <c r="P23" s="103"/>
-      <c r="Q23" s="103"/>
-      <c r="R23" s="103"/>
+      <c r="O23" s="101"/>
+      <c r="P23" s="101"/>
+      <c r="Q23" s="101"/>
+      <c r="R23" s="101"/>
       <c r="S23" s="28"/>
       <c r="Y23" s="28"/>
       <c r="Z23" s="28"/>
@@ -5564,17 +5511,17 @@
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="103"/>
+      <c r="H24" s="101"/>
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
+      <c r="O24" s="101"/>
+      <c r="P24" s="101"/>
+      <c r="Q24" s="101"/>
+      <c r="R24" s="101"/>
       <c r="S24" s="28"/>
       <c r="Y24" s="28"/>
       <c r="Z24" s="28"/>
@@ -5600,17 +5547,17 @@
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="103"/>
+      <c r="H25" s="101"/>
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="103"/>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="103"/>
+      <c r="O25" s="101"/>
+      <c r="P25" s="101"/>
+      <c r="Q25" s="101"/>
+      <c r="R25" s="101"/>
       <c r="S25" s="28"/>
       <c r="Y25" s="28"/>
       <c r="Z25" s="28"/>
@@ -5636,17 +5583,17 @@
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="103"/>
+      <c r="H26" s="101"/>
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
-      <c r="O26" s="103"/>
-      <c r="P26" s="103"/>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
+      <c r="O26" s="101"/>
+      <c r="P26" s="101"/>
+      <c r="Q26" s="101"/>
+      <c r="R26" s="101"/>
       <c r="S26" s="28"/>
       <c r="Y26" s="28"/>
       <c r="Z26" s="28"/>
@@ -5672,17 +5619,17 @@
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="103"/>
+      <c r="H27" s="101"/>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
-      <c r="O27" s="103"/>
-      <c r="P27" s="103"/>
-      <c r="Q27" s="103"/>
-      <c r="R27" s="103"/>
+      <c r="O27" s="101"/>
+      <c r="P27" s="101"/>
+      <c r="Q27" s="101"/>
+      <c r="R27" s="101"/>
       <c r="S27" s="28"/>
       <c r="Y27" s="28"/>
       <c r="Z27" s="28"/>
@@ -5708,17 +5655,17 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="103"/>
+      <c r="H28" s="101"/>
       <c r="I28" s="28"/>
       <c r="J28" s="28"/>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
-      <c r="O28" s="103"/>
-      <c r="P28" s="103"/>
-      <c r="Q28" s="103"/>
-      <c r="R28" s="103"/>
+      <c r="O28" s="101"/>
+      <c r="P28" s="101"/>
+      <c r="Q28" s="101"/>
+      <c r="R28" s="101"/>
       <c r="S28" s="28"/>
       <c r="Y28" s="28"/>
       <c r="Z28" s="28"/>
@@ -5744,17 +5691,17 @@
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="103"/>
+      <c r="H29" s="101"/>
       <c r="I29" s="28"/>
       <c r="J29" s="28"/>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
       <c r="M29" s="22"/>
       <c r="N29" s="22"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
+      <c r="O29" s="101"/>
+      <c r="P29" s="101"/>
+      <c r="Q29" s="101"/>
+      <c r="R29" s="101"/>
       <c r="S29" s="28"/>
       <c r="Y29" s="28"/>
       <c r="Z29" s="28"/>
@@ -5780,17 +5727,17 @@
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
       <c r="G30" s="21"/>
-      <c r="H30" s="103"/>
+      <c r="H30" s="101"/>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
+      <c r="O30" s="101"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="101"/>
       <c r="S30" s="28"/>
       <c r="Y30" s="28"/>
       <c r="Z30" s="28"/>
@@ -5816,17 +5763,17 @@
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="103"/>
+      <c r="H31" s="101"/>
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
       <c r="M31" s="22"/>
       <c r="N31" s="22"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
+      <c r="O31" s="101"/>
+      <c r="P31" s="101"/>
+      <c r="Q31" s="101"/>
+      <c r="R31" s="101"/>
       <c r="S31" s="28"/>
       <c r="Y31" s="28"/>
       <c r="Z31" s="28"/>
@@ -10218,11 +10165,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BC1000"/>
+  <dimension ref="A1:AH1000"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10236,197 +10183,159 @@
     <col min="7" max="7" width="9.6640625" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" style="28" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="17.1640625" style="28" customWidth="1"/>
-    <col min="24" max="16384" width="14.5" style="28"/>
+    <col min="10" max="10" width="9.5" style="28" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="28" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.83203125" style="28" customWidth="1"/>
+    <col min="18" max="27" width="8.33203125" style="28" customWidth="1"/>
+    <col min="28" max="28" width="16.83203125" style="28" customWidth="1"/>
+    <col min="29" max="16384" width="14.5" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:34" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="115" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="116" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="116" t="s">
+        <v>230</v>
+      </c>
+      <c r="K1" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="116" t="s">
+        <v>237</v>
+      </c>
+      <c r="M1" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="115" t="s">
+        <v>115</v>
+      </c>
+      <c r="P1" s="115" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="N1" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="48" t="s">
+      <c r="Q1" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="R1" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="R1" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="T1" s="47" t="s">
+      <c r="S1" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="T1" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="47" t="s">
+      <c r="U1" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="47" t="s">
+      <c r="V1" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="47" t="s">
+      <c r="W1" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="47" t="s">
+      <c r="X1" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="47" t="s">
+      <c r="Y1" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="47" t="s">
+      <c r="Z1" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="47" t="s">
+      <c r="AA1" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD1" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE1" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF1" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG1" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="AH1" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="AI1" s="43" t="s">
+      <c r="AB1" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="19"/>
-      <c r="AY1" s="19"/>
-      <c r="AZ1" s="19"/>
-      <c r="BA1" s="19"/>
-      <c r="BB1" s="19"/>
-      <c r="BC1" s="19"/>
-    </row>
-    <row r="2" spans="1:55" ht="84" x14ac:dyDescent="0.15">
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+    </row>
+    <row r="2" spans="1:34" ht="70" x14ac:dyDescent="0.15">
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
-      <c r="E2" s="106" t="s">
-        <v>115</v>
-      </c>
-      <c r="O2" s="106" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+      <c r="E2" s="104" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="104"/>
+    </row>
+    <row r="3" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:55" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:34" ht="13" x14ac:dyDescent="0.15">
       <c r="E16" s="21"/>
     </row>
     <row r="17" spans="5:5" ht="13" x14ac:dyDescent="0.15">
@@ -13382,7 +13291,7 @@
       <c r="E1000" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OO62Io7n8UvYOirx+yk6b9yZtH7tqdJq6QqUGu6eEurHXak6x9+6gYZNrBfCnEacEf+N1bdkFbAuBchiUPRLPQ==" saltValue="OLeOZFW2TH7lWMIeyrzR5g==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" sort="0" autoFilter="0"/>
   <phoneticPr fontId="16" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -13432,7 +13341,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" s="42" t="s">
         <v>11</v>
@@ -13444,43 +13353,43 @@
         <v>20</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="G1" s="42" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="I1" s="42" t="s">
         <v>42</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="K1" s="42" t="s">
         <v>43</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="M1" s="43" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="O1" s="43" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="P1" s="43" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="Q1" s="43" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="R1" s="43" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="S1" s="42" t="s">
         <v>3</v>
@@ -13514,16 +13423,16 @@
     <row r="2" spans="1:44" ht="56" x14ac:dyDescent="0.15">
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
-      <c r="E2" s="106" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="106" t="s">
-        <v>236</v>
+      <c r="E2" s="104" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="104" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:44" ht="13" x14ac:dyDescent="0.15">
@@ -16547,32 +16456,32 @@
     <col min="2" max="2" width="32.5" style="20" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" style="20" customWidth="1"/>
     <col min="4" max="4" width="56" style="29" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="66"/>
+    <col min="5" max="16384" width="14.5" style="65"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="35" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="108" t="s">
-        <v>226</v>
+      <c r="A2" s="106" t="s">
+        <v>203</v>
       </c>
       <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="108" t="s">
-        <v>187</v>
+      <c r="A3" s="106" t="s">
+        <v>172</v>
       </c>
       <c r="B3" s="30"/>
     </row>
@@ -16705,7 +16614,7 @@
     <row r="32" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B32" s="32"/>
       <c r="C32" s="25"/>
-      <c r="D32" s="109"/>
+      <c r="D32" s="107"/>
     </row>
     <row r="33" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B33" s="32"/>
@@ -17256,7 +17165,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17267,17 +17176,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>